<commit_message>
added a second task and buttons
</commit_message>
<xml_diff>
--- a/homework_data.xlsx
+++ b/homework_data.xlsx
@@ -1,26 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12300"/>
-  </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames/>
+  <calcPr/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="DkB2r0zp6u0Ko0gKEYuSC7bFM2HRUbj9OIVCGgzQYDA="/>
     </ext>
   </extLst>
 </workbook>
@@ -62,7 +51,7 @@
     <t>Колледж</t>
   </si>
   <si>
-    <t>Бибиджон Кира Алексеевна</t>
+    <t>Гончарова Кира Алексеевна</t>
   </si>
   <si>
     <t>Лукьянова Елена Сергеевна</t>
@@ -80,7 +69,7 @@
     <t>Суворова Маргарита</t>
   </si>
   <si>
-    <t>Ёмаё Павел</t>
+    <t>Трофимов Павел</t>
   </si>
   <si>
     <t>Хоменко Евгения</t>
@@ -92,902 +81,56 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="9">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
+  <borders count="1">
+    <border/>
   </borders>
-  <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Запятая" xfId="1" builtinId="3"/>
-    <cellStyle name="Денежный" xfId="2" builtinId="4"/>
-    <cellStyle name="Процент" xfId="3" builtinId="5"/>
-    <cellStyle name="Запятая [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Денежный [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Гиперссылка" xfId="6" builtinId="8"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="7" builtinId="9"/>
-    <cellStyle name="Примечание" xfId="8" builtinId="10"/>
-    <cellStyle name="Предупреждающий текст" xfId="9" builtinId="11"/>
-    <cellStyle name="Заголовок" xfId="10" builtinId="15"/>
-    <cellStyle name="Пояснительный текст" xfId="11" builtinId="53"/>
-    <cellStyle name="Заголовок 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Заголовок 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Заголовок 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Заголовок 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Ввод" xfId="16" builtinId="20"/>
-    <cellStyle name="Вывод" xfId="17" builtinId="21"/>
-    <cellStyle name="Вычисление" xfId="18" builtinId="22"/>
-    <cellStyle name="Проверить ячейку" xfId="19" builtinId="23"/>
-    <cellStyle name="Связанная ячейка" xfId="20" builtinId="24"/>
-    <cellStyle name="Итого" xfId="21" builtinId="25"/>
-    <cellStyle name="Хороший" xfId="22" builtinId="26"/>
-    <cellStyle name="Плохой" xfId="23" builtinId="27"/>
-    <cellStyle name="Нейтральный" xfId="24" builtinId="28"/>
-    <cellStyle name="Акцент1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% — Акцент1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% — Акцент1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% — Акцент1" xfId="28" builtinId="32"/>
-    <cellStyle name="Акцент2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% — Акцент2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% — Акцент2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% — Акцент2" xfId="32" builtinId="36"/>
-    <cellStyle name="Акцент3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% — Акцент3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% — Акцент3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% — Акцент3" xfId="36" builtinId="40"/>
-    <cellStyle name="Акцент4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% — Акцент4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% — Акцент4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% — Акцент4" xfId="40" builtinId="44"/>
-    <cellStyle name="Акцент5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% — Акцент5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% — Акцент5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% — Акцент5" xfId="44" builtinId="48"/>
-    <cellStyle name="Акцент6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% — Акцент6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% — Акцент6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% — Акцент6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="double">
-          <color theme="4"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <horizontal style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-  </dxfs>
-  <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
-    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="lastColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
-    </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="totalRow" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
-      <tableStyleElement type="pageFieldValues" dxfId="7"/>
-    </tableStyle>
-  </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <dxfs count="0"/>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1177,41 +320,39 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:Q1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="25.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="10.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="8.14285714285714" customWidth="1"/>
-    <col min="5" max="5" width="9.71428571428571" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="8.42857142857143" customWidth="1"/>
-    <col min="8" max="8" width="10.8571428571429" customWidth="1"/>
-    <col min="9" max="9" width="8.71428571428571" customWidth="1"/>
-    <col min="10" max="10" width="9.71428571428571" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="8.71428571428571" customWidth="1"/>
-    <col min="13" max="13" width="10.8571428571429" customWidth="1"/>
-    <col min="14" max="14" width="8.14285714285714" customWidth="1"/>
-    <col min="15" max="15" width="9.71428571428571" customWidth="1"/>
-    <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="26" width="8.71428571428571" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="16.14"/>
+    <col customWidth="1" min="2" max="2" width="25.86"/>
+    <col customWidth="1" min="3" max="3" width="10.86"/>
+    <col customWidth="1" min="4" max="4" width="8.14"/>
+    <col customWidth="1" min="5" max="5" width="9.71"/>
+    <col customWidth="1" min="6" max="6" width="11.0"/>
+    <col customWidth="1" min="7" max="7" width="8.43"/>
+    <col customWidth="1" min="8" max="8" width="10.86"/>
+    <col customWidth="1" min="9" max="9" width="8.71"/>
+    <col customWidth="1" min="10" max="10" width="9.71"/>
+    <col customWidth="1" min="11" max="11" width="11.0"/>
+    <col customWidth="1" min="12" max="12" width="8.71"/>
+    <col customWidth="1" min="13" max="13" width="10.86"/>
+    <col customWidth="1" min="14" max="14" width="8.14"/>
+    <col customWidth="1" min="15" max="15" width="9.71"/>
+    <col customWidth="1" min="16" max="16" width="11.0"/>
+    <col customWidth="1" min="17" max="26" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1" spans="1:13">
+    <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1228,7 +369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1" spans="3:17">
+    <row r="2" ht="14.25" customHeight="1">
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1275,7 +416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1" spans="1:12">
+    <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1283,317 +424,317 @@
         <v>11</v>
       </c>
       <c r="C3" s="1">
-        <v>74</v>
+        <v>74.0</v>
       </c>
       <c r="D3" s="1">
-        <v>476</v>
+        <v>476.0</v>
       </c>
       <c r="E3" s="1">
-        <v>335</v>
+        <v>335.0</v>
       </c>
       <c r="F3" s="1">
-        <v>335</v>
+        <v>335.0</v>
       </c>
       <c r="G3" s="1">
-        <v>1798</v>
+        <v>1798.0</v>
       </c>
       <c r="H3" s="1">
-        <v>20</v>
+        <v>20.0</v>
       </c>
       <c r="I3" s="1">
-        <v>108</v>
+        <v>108.0</v>
       </c>
       <c r="J3" s="1">
-        <v>131</v>
+        <v>131.0</v>
       </c>
       <c r="K3" s="1">
-        <v>131</v>
+        <v>131.0</v>
       </c>
       <c r="L3" s="1">
-        <v>438</v>
+        <v>438.0</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1" spans="2:12">
+    <row r="4" ht="14.25" customHeight="1">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="1">
-        <v>16</v>
+        <v>16.0</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="E4" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G4" s="1">
-        <v>239</v>
+        <v>239.0</v>
       </c>
       <c r="H4" s="1">
-        <v>8</v>
+        <v>8.0</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="K4" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="L4" s="1">
-        <v>120</v>
+        <v>120.0</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1" spans="2:12">
+    <row r="5" ht="14.25" customHeight="1">
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1">
-        <v>31</v>
+        <v>31.0</v>
       </c>
       <c r="D5" s="1">
-        <v>171</v>
+        <v>171.0</v>
       </c>
       <c r="E5" s="1">
-        <v>120</v>
+        <v>120.0</v>
       </c>
       <c r="F5" s="1">
-        <v>120</v>
+        <v>120.0</v>
       </c>
       <c r="G5" s="1">
-        <v>599</v>
+        <v>599.0</v>
       </c>
       <c r="H5" s="1">
-        <v>7</v>
+        <v>7.0</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="J5" s="1">
-        <v>32</v>
+        <v>32.0</v>
       </c>
       <c r="K5" s="1">
-        <v>32</v>
+        <v>32.0</v>
       </c>
       <c r="L5" s="1">
-        <v>110</v>
+        <v>110.0</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1" spans="2:12">
+    <row r="6" ht="14.25" customHeight="1">
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="1">
-        <v>61</v>
+        <v>61.0</v>
       </c>
       <c r="D6" s="1">
-        <v>536</v>
+        <v>536.0</v>
       </c>
       <c r="E6" s="1">
-        <v>620</v>
+        <v>620.0</v>
       </c>
       <c r="F6" s="1">
-        <v>620</v>
+        <v>620.0</v>
       </c>
       <c r="G6" s="1">
-        <v>1065</v>
+        <v>1065.0</v>
       </c>
       <c r="H6" s="1">
-        <v>11</v>
+        <v>11.0</v>
       </c>
       <c r="I6" s="1">
-        <v>106</v>
+        <v>106.0</v>
       </c>
       <c r="J6" s="1">
-        <v>194</v>
+        <v>194.0</v>
       </c>
       <c r="K6" s="1">
-        <v>194</v>
+        <v>194.0</v>
       </c>
       <c r="L6" s="1">
-        <v>241</v>
+        <v>241.0</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1" spans="2:12">
+    <row r="7" ht="14.25" customHeight="1">
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="1">
-        <v>76</v>
+        <v>76.0</v>
       </c>
       <c r="D7" s="1">
-        <v>813</v>
+        <v>813.0</v>
       </c>
       <c r="E7" s="1">
-        <v>732</v>
+        <v>732.0</v>
       </c>
       <c r="F7" s="1">
-        <v>732</v>
+        <v>732.0</v>
       </c>
       <c r="G7" s="1">
-        <v>1422</v>
+        <v>1422.0</v>
       </c>
       <c r="H7" s="1">
-        <v>20</v>
+        <v>20.0</v>
       </c>
       <c r="I7" s="1">
-        <v>187</v>
+        <v>187.0</v>
       </c>
       <c r="J7" s="1">
-        <v>273</v>
+        <v>273.0</v>
       </c>
       <c r="K7" s="1">
-        <v>273</v>
+        <v>273.0</v>
       </c>
       <c r="L7" s="1">
-        <v>404</v>
+        <v>404.0</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1" spans="2:12">
+    <row r="8" ht="14.25" customHeight="1">
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="1">
-        <v>33</v>
+        <v>33.0</v>
       </c>
       <c r="D8" s="1">
-        <v>308</v>
+        <v>308.0</v>
       </c>
       <c r="E8" s="1">
-        <v>231</v>
+        <v>231.0</v>
       </c>
       <c r="F8" s="1">
-        <v>231</v>
+        <v>231.0</v>
       </c>
       <c r="G8" s="1">
-        <v>592</v>
+        <v>592.0</v>
       </c>
       <c r="H8" s="1">
-        <v>11</v>
+        <v>11.0</v>
       </c>
       <c r="I8" s="1">
-        <v>127</v>
+        <v>127.0</v>
       </c>
       <c r="J8" s="1">
-        <v>84</v>
+        <v>84.0</v>
       </c>
       <c r="K8" s="1">
-        <v>84</v>
+        <v>84.0</v>
       </c>
       <c r="L8" s="1">
-        <v>250</v>
+        <v>250.0</v>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1" spans="2:12">
+    <row r="9" ht="14.25" customHeight="1">
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="1">
-        <v>42</v>
+        <v>42.0</v>
       </c>
       <c r="D9" s="1">
-        <v>500</v>
+        <v>500.0</v>
       </c>
       <c r="E9" s="1">
-        <v>296</v>
+        <v>296.0</v>
       </c>
       <c r="F9" s="1">
-        <v>296</v>
+        <v>296.0</v>
       </c>
       <c r="G9" s="1">
-        <v>941</v>
+        <v>941.0</v>
       </c>
       <c r="H9" s="1">
-        <v>11</v>
+        <v>11.0</v>
       </c>
       <c r="I9" s="1">
-        <v>195</v>
+        <v>195.0</v>
       </c>
       <c r="J9" s="1">
-        <v>171</v>
+        <v>171.0</v>
       </c>
       <c r="K9" s="1">
-        <v>171</v>
+        <v>171.0</v>
       </c>
       <c r="L9" s="1">
-        <v>266</v>
+        <v>266.0</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1" spans="2:12">
+    <row r="10" ht="14.25" customHeight="1">
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="1">
-        <v>90</v>
+        <v>90.0</v>
       </c>
       <c r="D10" s="1">
-        <v>1411</v>
+        <v>1411.0</v>
       </c>
       <c r="E10" s="1">
-        <v>950</v>
+        <v>950.0</v>
       </c>
       <c r="F10" s="1">
-        <v>950</v>
+        <v>950.0</v>
       </c>
       <c r="G10" s="1">
-        <v>1587</v>
+        <v>1587.0</v>
       </c>
       <c r="H10" s="1">
-        <v>22</v>
+        <v>22.0</v>
       </c>
       <c r="I10" s="1">
-        <v>341</v>
+        <v>341.0</v>
       </c>
       <c r="J10" s="1">
-        <v>372</v>
+        <v>372.0</v>
       </c>
       <c r="K10" s="1">
-        <v>372</v>
+        <v>372.0</v>
       </c>
       <c r="L10" s="1">
-        <v>415</v>
+        <v>415.0</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1" spans="2:12">
+    <row r="11" ht="14.25" customHeight="1">
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="1">
-        <v>8</v>
+        <v>8.0</v>
       </c>
       <c r="D11" s="1">
-        <v>75</v>
+        <v>75.0</v>
       </c>
       <c r="E11" s="1">
-        <v>55</v>
+        <v>55.0</v>
       </c>
       <c r="F11" s="1">
-        <v>55</v>
+        <v>55.0</v>
       </c>
       <c r="G11" s="1">
-        <v>138</v>
+        <v>138.0</v>
       </c>
       <c r="H11" s="1">
-        <v>3</v>
+        <v>3.0</v>
       </c>
       <c r="I11" s="1">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="J11" s="1">
-        <v>18</v>
+        <v>18.0</v>
       </c>
       <c r="K11" s="1">
-        <v>18</v>
+        <v>18.0</v>
       </c>
       <c r="L11" s="1">
-        <v>54</v>
+        <v>54.0</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1" spans="7:7">
+    <row r="12" ht="14.25" customHeight="1">
       <c r="G12" s="2"/>
     </row>
     <row r="13" ht="14.25" customHeight="1"/>
@@ -2586,15 +1727,16 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="A3:A11"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="1" orientation="landscape"/>
-  <headerFooter/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>